<commit_message>
- Updated meeting minutes - Updated sprint hours
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours .xlsx
+++ b/Meeting Minutes/SprintHours .xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\GITT\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Related Folders\University Work\Final Year Assignments\Group Project\Group 1\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="216">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -611,22 +611,73 @@
     <t>Bug fixes, Animation fixes, Play testing</t>
   </si>
   <si>
-    <t>EasterBreak</t>
-  </si>
-  <si>
-    <t>Added a more meaningful way of ending the memory</t>
-  </si>
-  <si>
-    <t>Added doors</t>
-  </si>
-  <si>
-    <t>Add more puzzles to the game play loop + Keep the player coming back to the notice Board</t>
+    <t>22/3/17 - 29/3/17</t>
+  </si>
+  <si>
+    <t>29/3/17 - 19/4/17</t>
+  </si>
+  <si>
+    <t>As a coder, make a variable which the game will update to see how many puzzle boards the player must do</t>
+  </si>
+  <si>
+    <t>As a coder, make the player turn to the carer when she catches you</t>
+  </si>
+  <si>
+    <t>As a sound artist, find sobbing sound effect for the player</t>
+  </si>
+  <si>
+    <t>As a user, update objects ingame</t>
+  </si>
+  <si>
+    <t>As a coder, implement a short sprint players can do</t>
+  </si>
+  <si>
+    <t>As a group, have some people playtest</t>
+  </si>
+  <si>
+    <t>As a modeler, texture the carer</t>
+  </si>
+  <si>
+    <t>As a modeler, look into potentially using Substance Painter 2</t>
+  </si>
+  <si>
+    <t>As a designer, fix the flickering dynamic lights</t>
+  </si>
+  <si>
+    <t>As a designer, find another cup image and a image of a vinyl record for the puzzle box</t>
+  </si>
+  <si>
+    <t>As a designer, figure out a way for the player to know a technique to solving the puzzle box</t>
+  </si>
+  <si>
+    <t>As a designer, create notes telling the player what the puzzle board looks like</t>
+  </si>
+  <si>
+    <t>As a sound artist, find some ambient sound effects for when the carer is cleaning the house</t>
+  </si>
+  <si>
+    <t>As a designer, create some dialogue lines for the carer</t>
+  </si>
+  <si>
+    <t>As a designer, look into getting a voice actor for the carer</t>
+  </si>
+  <si>
+    <t>As a designer, fix the main menu icons going small in full screen</t>
+  </si>
+  <si>
+    <t>As a coder, fix the puzzle box squares hiding the text prompt</t>
+  </si>
+  <si>
+    <t>As a modeler, texture the cooker</t>
+  </si>
+  <si>
+    <t>As a modeler, texture the record player</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1003,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J354"/>
+  <dimension ref="C3:J367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D342" sqref="D342"/>
+    <sheetView tabSelected="1" topLeftCell="B334" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E355" sqref="E355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3995,7 +4046,7 @@
     </row>
     <row r="321" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C321" s="1" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="D321" s="1"/>
       <c r="E321" s="1"/>
@@ -4060,11 +4111,13 @@
       <c r="D327" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E327" s="1"/>
+      <c r="E327" s="1">
+        <v>1</v>
+      </c>
       <c r="F327" s="1"/>
       <c r="G327" s="1">
         <f>E327+E328+E329+E330</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="328" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4072,7 +4125,9 @@
       <c r="D328" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E328" s="1"/>
+      <c r="E328" s="1">
+        <v>1</v>
+      </c>
       <c r="F328" s="1"/>
     </row>
     <row r="329" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4080,7 +4135,9 @@
       <c r="D329" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E329" s="1"/>
+      <c r="E329" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F329" s="1"/>
     </row>
     <row r="330" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4088,7 +4145,9 @@
       <c r="D330" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E330" s="1"/>
+      <c r="E330" s="1">
+        <v>4</v>
+      </c>
       <c r="F330" s="1"/>
     </row>
     <row r="331" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4104,11 +4163,13 @@
       <c r="D332" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E332" s="1"/>
+      <c r="E332" s="1">
+        <v>1</v>
+      </c>
       <c r="F332" s="1"/>
       <c r="G332" s="1">
         <f>E332+E333+E334+E335</f>
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="333" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4116,7 +4177,9 @@
       <c r="D333" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E333" s="1"/>
+      <c r="E333" s="1">
+        <v>1</v>
+      </c>
       <c r="F333" s="1"/>
     </row>
     <row r="334" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4124,7 +4187,9 @@
       <c r="D334" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E334" s="1"/>
+      <c r="E334" s="1">
+        <v>1</v>
+      </c>
       <c r="F334" s="1"/>
     </row>
     <row r="335" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4132,109 +4197,120 @@
       <c r="D335" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E335" s="1"/>
+      <c r="E335" s="1">
+        <v>2.5</v>
+      </c>
       <c r="F335" s="1"/>
     </row>
-    <row r="336" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="337" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="336" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="337" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C337" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D337" s="1"/>
+      <c r="E337" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F337" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G337" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="338" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C338" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D338" s="1"/>
+      <c r="E338" s="1"/>
+      <c r="F338" s="1">
+        <v>22</v>
+      </c>
+      <c r="G338" s="1">
+        <f>E339+E340+E341+E342+E343+E344+E345</f>
         <v>0</v>
-      </c>
-      <c r="D338" s="1"/>
-      <c r="E338" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F338" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G338" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="339" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C339" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D339" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="E339" s="1"/>
       <c r="F339" s="1"/>
-      <c r="G339" s="1">
-        <f>E340+E341+E342+E343+E344</f>
-        <v>16</v>
-      </c>
     </row>
     <row r="340" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C340" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C340" s="1"/>
       <c r="D340" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E340" s="1">
-        <v>10</v>
-      </c>
+      <c r="E340" s="1"/>
       <c r="F340" s="1"/>
     </row>
     <row r="341" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C341" s="1"/>
       <c r="D341" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E341" s="1">
-        <v>1</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="E341" s="1"/>
       <c r="F341" s="1"/>
     </row>
     <row r="342" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C342" s="1"/>
       <c r="D342" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E342" s="1">
-        <v>5</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="E342" s="1"/>
       <c r="F342" s="1"/>
     </row>
     <row r="343" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C343" s="1"/>
-      <c r="D343" s="1"/>
+      <c r="D343" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="E343" s="1"/>
       <c r="F343" s="1"/>
     </row>
     <row r="344" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C344" s="1"/>
-      <c r="D344" s="1"/>
+      <c r="D344" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="E344" s="1"/>
       <c r="F344" s="1"/>
     </row>
     <row r="345" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C345" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D345" s="1"/>
+      <c r="C345" s="1"/>
+      <c r="D345" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="E345" s="1"/>
       <c r="F345" s="1"/>
-      <c r="G345" s="1">
-        <f>E345+E346+E347+E348</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="346" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C346" s="1"/>
-      <c r="D346" s="1"/>
+      <c r="D346" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="E346" s="1"/>
       <c r="F346" s="1"/>
     </row>
     <row r="347" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C347" s="1"/>
-      <c r="D347" s="1"/>
+      <c r="D347" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="E347" s="1"/>
       <c r="F347" s="1"/>
     </row>
     <row r="348" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C348" s="1"/>
-      <c r="D348" s="1"/>
+      <c r="D348" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="E348" s="1"/>
       <c r="F348" s="1"/>
     </row>
@@ -4246,35 +4322,161 @@
     </row>
     <row r="350" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C350" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D350" s="1"/>
-      <c r="E350" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E350" s="1">
+        <v>1</v>
+      </c>
       <c r="F350" s="1"/>
       <c r="G350" s="1">
-        <f>E350+E351+E352+E353</f>
-        <v>0</v>
+        <f>E359+E353+E354+E355+E356+E357+E358+E352+E351+E350+E360</f>
+        <v>4.5</v>
       </c>
     </row>
     <row r="351" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C351" s="1"/>
-      <c r="D351" s="1"/>
+      <c r="D351" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="E351" s="1"/>
       <c r="F351" s="1"/>
     </row>
     <row r="352" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C352" s="1"/>
-      <c r="D352" s="1"/>
+      <c r="D352" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="E352" s="1"/>
       <c r="F352" s="1"/>
     </row>
-    <row r="353" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C353" s="1"/>
-      <c r="D353" s="1"/>
+      <c r="D353" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="E353" s="1"/>
       <c r="F353" s="1"/>
     </row>
-    <row r="354" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="354" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C354" s="1"/>
+      <c r="D354" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E354" s="1"/>
+      <c r="F354" s="1"/>
+    </row>
+    <row r="355" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C355" s="1"/>
+      <c r="D355" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E355" s="1"/>
+      <c r="F355" s="1"/>
+    </row>
+    <row r="356" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C356" s="1"/>
+      <c r="D356" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E356" s="1">
+        <v>1</v>
+      </c>
+      <c r="F356" s="1"/>
+    </row>
+    <row r="357" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C357" s="1"/>
+      <c r="D357" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E357" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F357" s="1"/>
+    </row>
+    <row r="358" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C358" s="1"/>
+      <c r="D358" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E358" s="1">
+        <v>1</v>
+      </c>
+      <c r="F358" s="1"/>
+    </row>
+    <row r="359" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C359" s="1"/>
+      <c r="D359" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E359" s="1"/>
+      <c r="F359" s="1"/>
+    </row>
+    <row r="360" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C360" s="1"/>
+      <c r="D360" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E360" s="1">
+        <v>1</v>
+      </c>
+      <c r="F360" s="1"/>
+    </row>
+    <row r="361" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C361" s="1"/>
+      <c r="D361" s="1"/>
+      <c r="E361" s="1"/>
+      <c r="F361" s="1"/>
+    </row>
+    <row r="362" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C362" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E362" s="1"/>
+      <c r="F362" s="1"/>
+      <c r="G362" s="1">
+        <f>E362+E363+E364+E365+E366</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C363" s="1"/>
+      <c r="D363" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E363" s="1"/>
+      <c r="F363" s="1"/>
+    </row>
+    <row r="364" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C364" s="1"/>
+      <c r="D364" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E364" s="1"/>
+      <c r="F364" s="1"/>
+    </row>
+    <row r="365" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C365" s="1"/>
+      <c r="D365" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E365" s="1"/>
+      <c r="F365" s="1"/>
+    </row>
+    <row r="366" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C366" s="1"/>
+      <c r="D366" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E366" s="1"/>
+      <c r="F366" s="1"/>
+    </row>
+    <row r="367" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
- Added to meeting minutes - Added to sprint hours - Added new file: Presentation final
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours .xlsx
+++ b/Meeting Minutes/SprintHours .xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\GITT\Meeting Minutes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Related Folders\University Work\Final Year Assignments\Group Project\Group 1\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="218">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -675,12 +675,15 @@
   </si>
   <si>
     <t>Other Tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a group member, fix problems/tidy work </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1057,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:J368"/>
+  <dimension ref="C3:J369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B332" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G343" sqref="G343"/>
+    <sheetView tabSelected="1" topLeftCell="B344" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D374" sqref="D374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4358,8 +4361,8 @@
       </c>
       <c r="F351" s="1"/>
       <c r="G351" s="1">
-        <f>E360+E354+E355+E356+E357+E358+E359+E353+E352+E351+E361</f>
-        <v>4.5</v>
+        <f>E360+E354+E355+E356+E357+E358+E359+E353+E352+E351+E361+E362</f>
+        <v>10.5</v>
       </c>
     </row>
     <row r="352" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4367,7 +4370,9 @@
       <c r="D352" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E352" s="1"/>
+      <c r="E352" s="1">
+        <v>1.5</v>
+      </c>
       <c r="F352" s="1"/>
     </row>
     <row r="353" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4375,7 +4380,9 @@
       <c r="D353" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E353" s="1"/>
+      <c r="E353" s="1">
+        <v>0</v>
+      </c>
       <c r="F353" s="1"/>
     </row>
     <row r="354" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4383,7 +4390,9 @@
       <c r="D354" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E354" s="1"/>
+      <c r="E354" s="1">
+        <v>2</v>
+      </c>
       <c r="F354" s="1"/>
     </row>
     <row r="355" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4437,7 +4446,9 @@
       <c r="D360" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E360" s="1"/>
+      <c r="E360" s="1">
+        <v>0.5</v>
+      </c>
       <c r="F360" s="1"/>
     </row>
     <row r="361" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4452,36 +4463,38 @@
     </row>
     <row r="362" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C362" s="1"/>
-      <c r="D362" s="1"/>
-      <c r="E362" s="1"/>
+      <c r="D362" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E362" s="1">
+        <v>2</v>
+      </c>
       <c r="F362" s="1"/>
     </row>
     <row r="363" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C363" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D363" s="1" t="s">
-        <v>214</v>
-      </c>
+      <c r="C363" s="1"/>
+      <c r="D363" s="1"/>
       <c r="E363" s="1"/>
       <c r="F363" s="1"/>
-      <c r="G363" s="1">
-        <f>E363+E364+E365+E366+E367</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="364" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C364" s="1"/>
+      <c r="C364" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="D364" s="1" t="s">
-        <v>158</v>
+        <v>214</v>
       </c>
       <c r="E364" s="1"/>
       <c r="F364" s="1"/>
+      <c r="G364" s="1">
+        <f>E364+E365+E366+E367+E368</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="365" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C365" s="1"/>
       <c r="D365" s="1" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
       <c r="E365" s="1"/>
       <c r="F365" s="1"/>
@@ -4489,7 +4502,7 @@
     <row r="366" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C366" s="1"/>
       <c r="D366" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E366" s="1"/>
       <c r="F366" s="1"/>
@@ -4497,12 +4510,20 @@
     <row r="367" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C367" s="1"/>
       <c r="D367" s="1" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="E367" s="1"/>
       <c r="F367" s="1"/>
     </row>
-    <row r="368" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="368" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C368" s="1"/>
+      <c r="D368" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="E368" s="1"/>
+      <c r="F368" s="1"/>
+    </row>
+    <row r="369" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Minutes for this week
</commit_message>
<xml_diff>
--- a/Meeting Minutes/SprintHours .xlsx
+++ b/Meeting Minutes/SprintHours .xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Desktop\GroupGame\GameFiles\GITT\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="227">
   <si>
     <t xml:space="preserve">Group Member </t>
   </si>
@@ -687,12 +687,30 @@
   </si>
   <si>
     <t>Lee</t>
+  </si>
+  <si>
+    <t>29/3/17 - 26/4/17</t>
+  </si>
+  <si>
+    <t>Play Test Game</t>
+  </si>
+  <si>
+    <t>Incorperate Noticeboard Art</t>
+  </si>
+  <si>
+    <t>Make sure the gameplay loop is working correctly</t>
+  </si>
+  <si>
+    <t>Changes to positions of some puzzleboards</t>
+  </si>
+  <si>
+    <t>Make sure the noticeboard art changes after each completion of a puzzle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -773,7 +791,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1090,8 +1108,10 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -1132,7 +1152,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D172-4296-B89D-76E4880173F3}"/>
             </c:ext>
@@ -1803,7 +1823,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28C5380B-72B0-417A-B856-4908823361AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{28C5380B-72B0-417A-B856-4908823361AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1840,7 +1860,7 @@
         <cdr:cNvPr id="2" name="TextBox 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E024505E-BF05-43BF-879F-05E9D1051701}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E024505E-BF05-43BF-879F-05E9D1051701}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -2171,10 +2191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:K369"/>
+  <dimension ref="C3:K403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="A360" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D378" sqref="D378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5678,7 +5698,252 @@
       </c>
       <c r="F368" s="1"/>
     </row>
-    <row r="369" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="369" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="370" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="371" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C371" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D371" s="1"/>
+      <c r="E371" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F371" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G371" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="372" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C372" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D372" s="1"/>
+      <c r="E372" s="1"/>
+      <c r="F372" s="1">
+        <v>23</v>
+      </c>
+      <c r="G372" s="1">
+        <f>E373+E374+E375+E376+E377+E378+E379+E380+E381+E382+E383</f>
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="373" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C373" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E373" s="1">
+        <v>2</v>
+      </c>
+      <c r="F373" s="1"/>
+    </row>
+    <row r="374" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C374" s="1"/>
+      <c r="D374" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E374" s="1">
+        <v>1</v>
+      </c>
+      <c r="F374" s="1"/>
+    </row>
+    <row r="375" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C375" s="1"/>
+      <c r="D375" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E375" s="1">
+        <v>2</v>
+      </c>
+      <c r="F375" s="1"/>
+    </row>
+    <row r="376" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C376" s="1"/>
+      <c r="D376" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E376" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F376" s="1"/>
+    </row>
+    <row r="377" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C377" s="1"/>
+      <c r="D377" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E377" s="1">
+        <v>1</v>
+      </c>
+      <c r="F377" s="1"/>
+    </row>
+    <row r="378" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C378" s="1"/>
+      <c r="D378" s="1"/>
+      <c r="E378" s="1"/>
+      <c r="F378" s="1"/>
+    </row>
+    <row r="379" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C379" s="1"/>
+      <c r="D379" s="1"/>
+      <c r="E379" s="1"/>
+      <c r="F379" s="1"/>
+    </row>
+    <row r="380" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C380" s="1"/>
+      <c r="D380" s="1"/>
+      <c r="E380" s="1"/>
+      <c r="F380" s="1"/>
+    </row>
+    <row r="381" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C381" s="1"/>
+      <c r="D381" s="1"/>
+      <c r="E381" s="1"/>
+      <c r="F381" s="1"/>
+    </row>
+    <row r="382" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C382" s="1"/>
+      <c r="D382" s="1"/>
+      <c r="E382" s="1"/>
+      <c r="F382" s="1"/>
+    </row>
+    <row r="383" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C383" s="1"/>
+      <c r="D383" s="1"/>
+      <c r="E383" s="1"/>
+      <c r="F383" s="1"/>
+    </row>
+    <row r="384" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C384" s="1"/>
+      <c r="D384" s="1"/>
+      <c r="E384" s="1"/>
+      <c r="F384" s="1"/>
+    </row>
+    <row r="385" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C385" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D385" s="1"/>
+      <c r="E385" s="1"/>
+      <c r="F385" s="1"/>
+      <c r="G385" s="1">
+        <f>E394+E388+E389+E390+E391+E392+E393+E387+E386+E385+E395+E396</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C386" s="1"/>
+      <c r="D386" s="1"/>
+      <c r="E386" s="1"/>
+      <c r="F386" s="1"/>
+    </row>
+    <row r="387" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C387" s="1"/>
+      <c r="D387" s="1"/>
+      <c r="E387" s="1"/>
+      <c r="F387" s="1"/>
+    </row>
+    <row r="388" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C388" s="1"/>
+      <c r="D388" s="1"/>
+      <c r="E388" s="1"/>
+      <c r="F388" s="1"/>
+    </row>
+    <row r="389" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C389" s="1"/>
+      <c r="D389" s="1"/>
+      <c r="E389" s="1"/>
+      <c r="F389" s="1"/>
+    </row>
+    <row r="390" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C390" s="1"/>
+      <c r="D390" s="1"/>
+      <c r="E390" s="1"/>
+      <c r="F390" s="1"/>
+    </row>
+    <row r="391" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C391" s="1"/>
+      <c r="D391" s="1"/>
+      <c r="E391" s="1"/>
+      <c r="F391" s="1"/>
+    </row>
+    <row r="392" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C392" s="1"/>
+      <c r="D392" s="1"/>
+      <c r="E392" s="1"/>
+      <c r="F392" s="1"/>
+    </row>
+    <row r="393" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C393" s="1"/>
+      <c r="D393" s="1"/>
+      <c r="E393" s="1"/>
+      <c r="F393" s="1"/>
+    </row>
+    <row r="394" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C394" s="1"/>
+      <c r="D394" s="1"/>
+      <c r="E394" s="1"/>
+      <c r="F394" s="1"/>
+    </row>
+    <row r="395" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C395" s="1"/>
+      <c r="D395" s="1"/>
+      <c r="E395" s="1"/>
+      <c r="F395" s="1"/>
+    </row>
+    <row r="396" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C396" s="1"/>
+      <c r="D396" s="1"/>
+      <c r="E396" s="1"/>
+      <c r="F396" s="1"/>
+    </row>
+    <row r="397" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C397" s="1"/>
+      <c r="D397" s="1"/>
+      <c r="E397" s="1"/>
+      <c r="F397" s="1"/>
+    </row>
+    <row r="398" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C398" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D398" s="1"/>
+      <c r="E398" s="1"/>
+      <c r="F398" s="1"/>
+      <c r="G398" s="1">
+        <f>E398+E399+E400+E401+E402</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C399" s="1"/>
+      <c r="D399" s="1"/>
+      <c r="E399" s="1"/>
+      <c r="F399" s="1"/>
+    </row>
+    <row r="400" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C400" s="1"/>
+      <c r="D400" s="1"/>
+      <c r="E400" s="1"/>
+      <c r="F400" s="1"/>
+    </row>
+    <row r="401" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C401" s="1"/>
+      <c r="D401" s="1"/>
+      <c r="E401" s="1"/>
+      <c r="F401" s="1"/>
+    </row>
+    <row r="402" spans="3:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C402" s="1"/>
+      <c r="D402" s="1"/>
+      <c r="E402" s="1"/>
+      <c r="F402" s="1"/>
+    </row>
+    <row r="403" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>